<commit_message>
Added columns to tesst case report
</commit_message>
<xml_diff>
--- a/TestCaseFile/TestCases_Selenium_GUI.xlsx
+++ b/TestCaseFile/TestCases_Selenium_GUI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Persistent_Mini_Project\Team_One_Opencart\TestCaseFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TeamOne_Opencart\TestCaseFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3C8524-7CD4-44AC-ACE0-A152657D9DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96325CB9-8462-4885-93EB-CA88D0E2B24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Project Name:</t>
   </si>
@@ -82,23 +82,6 @@
   </si>
   <si>
     <t>Actual Result</t>
-  </si>
-  <si>
-    <t>AUT URL: http://localhost/ecommerce/index.php
-Email: test123@gmail.com
-Password: 12345</t>
-  </si>
-  <si>
-    <t>1. Enter Email in Email field.
-2. Password Email in Password field.
-3. Press "Log In" button to login.
-4.Order Product</t>
-  </si>
-  <si>
-    <t>1. Email is displayed in email field.
-2. Dots representing password characters are displayed in password field.
-3. Log In Button is clickable and loads user login.
-4.Product ordered successfully.</t>
   </si>
   <si>
     <t>OpenCart (Locally Hosted)</t>
@@ -175,6 +158,24 @@
   </si>
   <si>
     <t>VT_05</t>
+  </si>
+  <si>
+    <t>AJ_02</t>
+  </si>
+  <si>
+    <t>AJ_03</t>
+  </si>
+  <si>
+    <t>AJ_04</t>
+  </si>
+  <si>
+    <t>AJ_05</t>
+  </si>
+  <si>
+    <t>Module Name</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -349,7 +350,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -450,11 +451,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -615,6 +640,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -622,6 +653,47 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -904,141 +976,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10:L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.90625" customWidth="1"/>
-    <col min="2" max="2" width="81.7265625" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" customWidth="1"/>
-    <col min="4" max="4" width="24.81640625" customWidth="1"/>
-    <col min="5" max="5" width="20.453125" customWidth="1"/>
-    <col min="6" max="6" width="34.26953125" customWidth="1"/>
-    <col min="7" max="7" width="46.1796875" customWidth="1"/>
-    <col min="8" max="8" width="45.26953125" customWidth="1"/>
-    <col min="9" max="9" width="49.26953125" customWidth="1"/>
-    <col min="10" max="10" width="16.36328125" customWidth="1"/>
+    <col min="1" max="2" width="24.90625" customWidth="1"/>
+    <col min="3" max="3" width="81.7265625" customWidth="1"/>
+    <col min="4" max="4" width="25.1796875" customWidth="1"/>
+    <col min="5" max="5" width="24.81640625" customWidth="1"/>
+    <col min="6" max="6" width="20.453125" customWidth="1"/>
+    <col min="7" max="7" width="34.26953125" customWidth="1"/>
+    <col min="8" max="8" width="46.1796875" customWidth="1"/>
+    <col min="9" max="9" width="45.26953125" customWidth="1"/>
+    <col min="10" max="10" width="49.26953125" customWidth="1"/>
+    <col min="11" max="12" width="16.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="7"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="57"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="8"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="55"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="8"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J2" s="7"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="40"/>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="D3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="10"/>
       <c r="E3" s="10"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="10"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="41"/>
-      <c r="B4" s="10"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="8"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I4" s="11"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="42"/>
-      <c r="B5" s="12"/>
+      <c r="B5" s="61"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.35">
+      <c r="J5" s="13"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+    </row>
+    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="A6" s="43"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="43"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="65"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="14"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="62"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="66"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -1047,377 +1133,427 @@
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
+      <c r="B9" s="64"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="18"/>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="44" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="D10" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="E10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="F10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="G10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="H10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="I10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="J10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="K10" s="67" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="67.5" x14ac:dyDescent="0.35">
+      <c r="L10" s="73" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="21"/>
+        <v>23</v>
+      </c>
+      <c r="B11" s="20"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" s="20"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E11" s="21"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="68"/>
+      <c r="L11" s="74"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="21"/>
+        <v>28</v>
+      </c>
+      <c r="B12" s="20"/>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="20"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E12" s="21"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="68"/>
+      <c r="L12" s="74"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="21"/>
+        <v>29</v>
+      </c>
+      <c r="B13" s="20"/>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="23"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="23"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="20"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I13" s="23"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="74"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="21"/>
+        <v>30</v>
+      </c>
+      <c r="B14" s="20"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="23"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="23"/>
       <c r="I14" s="23"/>
-      <c r="J14" s="20"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J14" s="23"/>
+      <c r="K14" s="68"/>
+      <c r="L14" s="74"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="21"/>
+        <v>31</v>
+      </c>
+      <c r="B15" s="20"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="20"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="68"/>
+      <c r="L15" s="74"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="28"/>
-      <c r="B16" s="29"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="29"/>
       <c r="D16" s="29"/>
       <c r="E16" s="29"/>
-      <c r="F16" s="28"/>
+      <c r="F16" s="29"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="28"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H16" s="28"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="69"/>
+      <c r="L16" s="75"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="21"/>
+        <v>24</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="31"/>
       <c r="D17" s="21"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="23"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="32"/>
       <c r="I17" s="23"/>
-      <c r="J17" s="20"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J17" s="23"/>
+      <c r="K17" s="68"/>
+      <c r="L17" s="74"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="21"/>
+        <v>32</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="31"/>
       <c r="D18" s="21"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="23"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22"/>
       <c r="G18" s="23"/>
-      <c r="H18" s="24"/>
+      <c r="H18" s="23"/>
       <c r="I18" s="24"/>
-      <c r="J18" s="20"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J18" s="24"/>
+      <c r="K18" s="68"/>
+      <c r="L18" s="74"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="21"/>
+        <v>33</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="31"/>
       <c r="D19" s="21"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="23"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="22"/>
       <c r="G19" s="23"/>
       <c r="H19" s="23"/>
       <c r="I19" s="23"/>
-      <c r="J19" s="20"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J19" s="23"/>
+      <c r="K19" s="68"/>
+      <c r="L19" s="74"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="21"/>
+        <v>34</v>
+      </c>
+      <c r="B20" s="20"/>
       <c r="C20" s="21"/>
       <c r="D20" s="21"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="23"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="33"/>
       <c r="G20" s="23"/>
       <c r="H20" s="23"/>
       <c r="I20" s="23"/>
-      <c r="J20" s="20"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J20" s="23"/>
+      <c r="K20" s="68"/>
+      <c r="L20" s="74"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="21"/>
+        <v>35</v>
+      </c>
+      <c r="B21" s="20"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="23"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="33"/>
       <c r="G21" s="23"/>
       <c r="H21" s="23"/>
       <c r="I21" s="23"/>
-      <c r="J21" s="20"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J21" s="23"/>
+      <c r="K21" s="68"/>
+      <c r="L21" s="74"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="28"/>
-      <c r="B22" s="29"/>
+      <c r="B22" s="28"/>
       <c r="C22" s="29"/>
       <c r="D22" s="29"/>
       <c r="E22" s="29"/>
-      <c r="F22" s="28"/>
+      <c r="F22" s="29"/>
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
       <c r="I22" s="28"/>
       <c r="J22" s="28"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K22" s="69"/>
+      <c r="L22" s="75"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="21"/>
+        <v>25</v>
+      </c>
+      <c r="B23" s="20"/>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="23"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="23"/>
       <c r="I23" s="23"/>
-      <c r="J23" s="20"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J23" s="23"/>
+      <c r="K23" s="68"/>
+      <c r="L23" s="74"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="21"/>
+        <v>36</v>
+      </c>
+      <c r="B24" s="34"/>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="20"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="23"/>
       <c r="J24" s="20"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K24" s="68"/>
+      <c r="L24" s="74"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="21"/>
+        <v>38</v>
+      </c>
+      <c r="B25" s="20"/>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="23"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="25"/>
       <c r="G25" s="23"/>
       <c r="H25" s="23"/>
       <c r="I25" s="23"/>
-      <c r="J25" s="20"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J25" s="23"/>
+      <c r="K25" s="68"/>
+      <c r="L25" s="74"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="21"/>
+        <v>37</v>
+      </c>
+      <c r="B26" s="20"/>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="23"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="20"/>
       <c r="H26" s="23"/>
       <c r="I26" s="23"/>
-      <c r="J26" s="20"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J26" s="23"/>
+      <c r="K26" s="68"/>
+      <c r="L26" s="74"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="21"/>
+        <v>39</v>
+      </c>
+      <c r="B27" s="20"/>
       <c r="C27" s="21"/>
       <c r="D27" s="21"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="23"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="20"/>
       <c r="H27" s="23"/>
       <c r="I27" s="23"/>
-      <c r="J27" s="20"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J27" s="23"/>
+      <c r="K27" s="68"/>
+      <c r="L27" s="74"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="28"/>
-      <c r="B28" s="29"/>
+      <c r="B28" s="28"/>
       <c r="C28" s="29"/>
       <c r="D28" s="29"/>
       <c r="E28" s="29"/>
-      <c r="F28" s="28"/>
+      <c r="F28" s="29"/>
       <c r="G28" s="28"/>
       <c r="H28" s="28"/>
       <c r="I28" s="28"/>
       <c r="J28" s="28"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K28" s="69"/>
+      <c r="L28" s="75"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="21"/>
+        <v>26</v>
+      </c>
+      <c r="B29" s="20"/>
       <c r="C29" s="21"/>
       <c r="D29" s="21"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="23"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="20"/>
       <c r="H29" s="23"/>
       <c r="I29" s="23"/>
-      <c r="J29" s="20"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J29" s="23"/>
+      <c r="K29" s="68"/>
+      <c r="L29" s="74"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="21"/>
+        <v>44</v>
+      </c>
+      <c r="B30" s="20"/>
+      <c r="C30" s="31"/>
       <c r="D30" s="21"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="20"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="22"/>
       <c r="G30" s="20"/>
-      <c r="H30" s="23"/>
+      <c r="H30" s="20"/>
       <c r="I30" s="23"/>
-      <c r="J30" s="20"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J30" s="23"/>
+      <c r="K30" s="68"/>
+      <c r="L30" s="74"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="21"/>
+        <v>45</v>
+      </c>
+      <c r="B31" s="20"/>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="20"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="25"/>
       <c r="G31" s="20"/>
-      <c r="H31" s="23"/>
+      <c r="H31" s="20"/>
       <c r="I31" s="23"/>
-      <c r="J31" s="20"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J31" s="23"/>
+      <c r="K31" s="68"/>
+      <c r="L31" s="74"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="21"/>
+        <v>46</v>
+      </c>
+      <c r="B32" s="20"/>
       <c r="C32" s="21"/>
       <c r="D32" s="21"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="23"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="37"/>
       <c r="I32" s="23"/>
-      <c r="J32" s="20"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J32" s="23"/>
+      <c r="K32" s="68"/>
+      <c r="L32" s="74"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="46"/>
+        <v>47</v>
+      </c>
+      <c r="B33" s="45"/>
       <c r="C33" s="46"/>
       <c r="D33" s="46"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="45"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="47"/>
       <c r="G33" s="45"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="45"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="48"/>
       <c r="J33" s="45"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K33" s="70"/>
+      <c r="L33" s="74"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="51"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="53"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="52"/>
       <c r="D34" s="53"/>
       <c r="E34" s="53"/>
       <c r="F34" s="53"/>
@@ -1425,13 +1561,15 @@
       <c r="H34" s="53"/>
       <c r="I34" s="53"/>
       <c r="J34" s="53"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K34" s="71"/>
+      <c r="L34" s="53"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" s="49"/>
-      <c r="C35" s="50"/>
+        <v>27</v>
+      </c>
+      <c r="B35" s="42"/>
+      <c r="C35" s="49"/>
       <c r="D35" s="50"/>
       <c r="E35" s="50"/>
       <c r="F35" s="50"/>
@@ -1439,13 +1577,15 @@
       <c r="H35" s="50"/>
       <c r="I35" s="50"/>
       <c r="J35" s="50"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K35" s="72"/>
+      <c r="L35" s="50"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" s="49"/>
-      <c r="C36" s="50"/>
+        <v>40</v>
+      </c>
+      <c r="B36" s="42"/>
+      <c r="C36" s="49"/>
       <c r="D36" s="50"/>
       <c r="E36" s="50"/>
       <c r="F36" s="50"/>
@@ -1453,13 +1593,15 @@
       <c r="H36" s="50"/>
       <c r="I36" s="50"/>
       <c r="J36" s="50"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K36" s="72"/>
+      <c r="L36" s="50"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" s="49"/>
-      <c r="C37" s="50"/>
+        <v>41</v>
+      </c>
+      <c r="B37" s="42"/>
+      <c r="C37" s="49"/>
       <c r="D37" s="50"/>
       <c r="E37" s="50"/>
       <c r="F37" s="50"/>
@@ -1467,13 +1609,15 @@
       <c r="H37" s="50"/>
       <c r="I37" s="50"/>
       <c r="J37" s="50"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K37" s="72"/>
+      <c r="L37" s="50"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="49"/>
-      <c r="C38" s="50"/>
+        <v>42</v>
+      </c>
+      <c r="B38" s="42"/>
+      <c r="C38" s="49"/>
       <c r="D38" s="50"/>
       <c r="E38" s="50"/>
       <c r="F38" s="50"/>
@@ -1481,13 +1625,15 @@
       <c r="H38" s="50"/>
       <c r="I38" s="50"/>
       <c r="J38" s="50"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K38" s="72"/>
+      <c r="L38" s="50"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="49"/>
-      <c r="C39" s="50"/>
+        <v>43</v>
+      </c>
+      <c r="B39" s="42"/>
+      <c r="C39" s="49"/>
       <c r="D39" s="50"/>
       <c r="E39" s="50"/>
       <c r="F39" s="50"/>
@@ -1495,11 +1641,13 @@
       <c r="H39" s="50"/>
       <c r="I39" s="50"/>
       <c r="J39" s="50"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K39" s="72"/>
+      <c r="L39" s="50"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="42"/>
-      <c r="B40" s="49"/>
-      <c r="C40" s="50"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="49"/>
       <c r="D40" s="50"/>
       <c r="E40" s="50"/>
       <c r="F40" s="50"/>
@@ -1507,11 +1655,13 @@
       <c r="H40" s="50"/>
       <c r="I40" s="50"/>
       <c r="J40" s="50"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K40" s="72"/>
+      <c r="L40" s="50"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="42"/>
-      <c r="B41" s="49"/>
-      <c r="C41" s="50"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="49"/>
       <c r="D41" s="50"/>
       <c r="E41" s="50"/>
       <c r="F41" s="50"/>
@@ -1519,11 +1669,13 @@
       <c r="H41" s="50"/>
       <c r="I41" s="50"/>
       <c r="J41" s="50"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K41" s="72"/>
+      <c r="L41" s="50"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="42"/>
-      <c r="B42" s="49"/>
-      <c r="C42" s="50"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="49"/>
       <c r="D42" s="50"/>
       <c r="E42" s="50"/>
       <c r="F42" s="50"/>
@@ -1531,11 +1683,13 @@
       <c r="H42" s="50"/>
       <c r="I42" s="50"/>
       <c r="J42" s="50"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K42" s="72"/>
+      <c r="L42" s="50"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="50"/>
-      <c r="B43" s="49"/>
-      <c r="C43" s="50"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="49"/>
       <c r="D43" s="50"/>
       <c r="E43" s="50"/>
       <c r="F43" s="50"/>
@@ -1543,18 +1697,20 @@
       <c r="H43" s="50"/>
       <c r="I43" s="50"/>
       <c r="J43" s="50"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B45" s="1"/>
+      <c r="K43" s="72"/>
+      <c r="L43" s="50"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C45" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="C6:K6"/>
+    <mergeCell ref="C7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>